<commit_message>
add changes to hw results
</commit_message>
<xml_diff>
--- a/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
@@ -1299,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2537,8 +2537,8 @@
         <v>19</v>
       </c>
       <c r="E30">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>MIN(ROUNDUP(43*1.15,0),45)</f>
+        <v>45</v>
       </c>
       <c r="F30">
         <f>MIN(ROUNDUP(34*1.15,0),48)</f>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
small changes for homeworks
</commit_message>
<xml_diff>
--- a/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f361a4bc30e7aea/GitHub/AlexAmarioarei.github.io/Teaching/ProbabilityStatistics/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\ProbabilityStatistics\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1301,7 +1301,7 @@
   <dimension ref="A1:L134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1347,7 +1347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>2.3000000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>1.9000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>113</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>114</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>115</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>116</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>144</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>1.9000000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>122</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>124</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>125</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>126</v>
       </c>
@@ -6220,7 +6220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>127</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>128</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>129</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>130</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>131</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>132</v>
       </c>
@@ -6440,8 +6440,8 @@
         <v>244</v>
       </c>
       <c r="C123">
-        <f>MIN(ROUNDUP(0*1.1,0),78)</f>
-        <v>0</v>
+        <f>MIN(ROUNDUP(21*1.1,0),78)</f>
+        <v>24</v>
       </c>
       <c r="D123">
         <f t="shared" si="9"/>
@@ -6472,10 +6472,10 @@
       </c>
       <c r="L123">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>133</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>134</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>135</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>136</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>137</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>138</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>139</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>140</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>1.7000000000000002</v>
       </c>
     </row>
-    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>141</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>142</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -6952,7 +6952,7 @@
   <autoFilter ref="A1:L134">
     <filterColumn colId="1">
       <filters>
-        <filter val="241"/>
+        <filter val="244"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Adding the special homework for both courses
</commit_message>
<xml_diff>
--- a/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Tabel_Prob_Stat" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabel_Prob_Stat!$A$1:$L$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabel_Prob_Stat!$A$1:$K$134</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Nume</t>
   </si>
@@ -45,15 +45,9 @@
     <t>Tema_5</t>
   </si>
   <si>
-    <t>Tema_6</t>
-  </si>
-  <si>
     <t>Proiect_1</t>
   </si>
   <si>
-    <t>Proiect_2</t>
-  </si>
-  <si>
     <t>Examen</t>
   </si>
   <si>
@@ -457,6 +451,9 @@
   </si>
   <si>
     <t>CHIPER MARIUS DANIEL</t>
+  </si>
+  <si>
+    <t>Tema_Speciala</t>
   </si>
 </sst>
 </file>
@@ -1297,19 +1294,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:L134"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="25.1328125" customWidth="1"/>
+    <col min="7" max="8" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1332,24 +1329,21 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>12</v>
       </c>
       <c r="B2">
         <v>241</v>
@@ -1382,16 +1376,13 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <f>ROUNDUP(1+(C2/80+D2/20+E2/50+F2/50+G2/1+H2/1)/6*2.5,1)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C2/80+D2/20+E2/50+F2/50+G2/1)/5*2.5,1)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>241</v>
@@ -1424,16 +1415,13 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L66" si="0">ROUNDUP(1+(C3/80+D3/20+E3/50+F3/50+G3/1+H3/1)/6*2.5,1)</f>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C3/80+D3/20+E3/50+F3/50+G3/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>241</v>
@@ -1442,15 +1430,15 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D33" si="1">MIN(ROUNDUP(0*1.1,0),20)</f>
+        <f t="shared" ref="D4:D33" si="0">MIN(ROUNDUP(0*1.1,0),20)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E66" si="2">MIN(ROUNDUP(0*1.15,0),48)</f>
+        <f t="shared" ref="E4:E66" si="1">MIN(ROUNDUP(0*1.15,0),48)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F66" si="3">MIN(ROUNDUP(0*1.15,0),48)</f>
+        <f t="shared" ref="F4:F66" si="2">MIN(ROUNDUP(0*1.15,0),48)</f>
         <v>0</v>
       </c>
       <c r="G4">
@@ -1466,16 +1454,13 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C4/80+D4/20+E4/50+F4/50+G4/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>241</v>
@@ -1484,17 +1469,17 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
@@ -1508,16 +1493,13 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C5/80+D5/20+E5/50+F5/50+G5/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>241</v>
@@ -1534,7 +1516,7 @@
         <v>33</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G6">
@@ -1550,16 +1532,13 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C6/80+D6/20+E6/50+F6/50+G6/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>241</v>
@@ -1568,17 +1547,17 @@
         <v>0</v>
       </c>
       <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
@@ -1592,16 +1571,13 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C7/80+D7/20+E7/50+F7/50+G7/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>241</v>
@@ -1618,7 +1594,7 @@
         <v>30</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G8">
@@ -1634,16 +1610,13 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>1.9000000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C8/80+D8/20+E8/50+F8/50+G8/1)/5*2.5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>241</v>
@@ -1652,17 +1625,17 @@
         <v>59</v>
       </c>
       <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G9">
         <v>0</v>
       </c>
@@ -1676,16 +1649,13 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C9/80+D9/20+E9/50+F9/50+G9/1)/5*2.5,1)</f>
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>241</v>
@@ -1718,16 +1688,13 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C10/80+D10/20+E10/50+F10/50+G10/1)/5*2.5,1)</f>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>241</v>
@@ -1760,16 +1727,13 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C11/80+D11/20+E11/50+F11/50+G11/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>241</v>
@@ -1778,17 +1742,17 @@
         <v>58</v>
       </c>
       <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G12">
         <v>0</v>
       </c>
@@ -1802,16 +1766,13 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C12/80+D12/20+E12/50+F12/50+G12/1)/5*2.5,1)</f>
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>241</v>
@@ -1820,17 +1781,17 @@
         <v>0</v>
       </c>
       <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G13">
         <v>0</v>
       </c>
@@ -1844,16 +1805,13 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C13/80+D13/20+E13/50+F13/50+G13/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>241</v>
@@ -1862,17 +1820,17 @@
         <v>0</v>
       </c>
       <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G14">
         <v>0</v>
       </c>
@@ -1886,16 +1844,13 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C14/80+D14/20+E14/50+F14/50+G14/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>241</v>
@@ -1928,16 +1883,13 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C15/80+D15/20+E15/50+F15/50+G15/1)/5*2.5,1)</f>
+        <v>1.9000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>241</v>
@@ -1950,13 +1902,13 @@
         <v>15</v>
       </c>
       <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>0</v>
       </c>
@@ -1970,16 +1922,13 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C16/80+D16/20+E16/50+F16/50+G16/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>241</v>
@@ -2012,16 +1961,13 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C17/80+D17/20+E17/50+F17/50+G17/1)/5*2.5,1)</f>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>241</v>
@@ -2030,17 +1976,17 @@
         <v>0</v>
       </c>
       <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G18">
         <v>0</v>
       </c>
@@ -2054,16 +2000,13 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C18/80+D18/20+E18/50+F18/50+G18/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>241</v>
@@ -2096,16 +2039,13 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C19/80+D19/20+E19/50+F19/50+G19/1)/5*2.5,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>241</v>
@@ -2139,16 +2079,13 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C20/80+D20/20+E20/50+F20/50+G20/1)/5*2.5,1)</f>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>241</v>
@@ -2157,17 +2094,17 @@
         <v>55</v>
       </c>
       <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G21">
         <v>0</v>
       </c>
@@ -2181,16 +2118,13 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C21/80+D21/20+E21/50+F21/50+G21/1)/5*2.5,1)</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>241</v>
@@ -2199,17 +2133,17 @@
         <v>0</v>
       </c>
       <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G22">
         <v>0</v>
       </c>
@@ -2223,16 +2157,13 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C22/80+D22/20+E22/50+F22/50+G22/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>241</v>
@@ -2241,17 +2172,17 @@
         <v>0</v>
       </c>
       <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G23">
         <v>0</v>
       </c>
@@ -2265,16 +2196,13 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C23/80+D23/20+E23/50+F23/50+G23/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>241</v>
@@ -2283,17 +2211,17 @@
         <v>0</v>
       </c>
       <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G24">
         <v>0</v>
       </c>
@@ -2307,16 +2235,13 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C24/80+D24/20+E24/50+F24/50+G24/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>241</v>
@@ -2329,7 +2254,7 @@
         <v>20</v>
       </c>
       <c r="E25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F25">
@@ -2349,16 +2274,13 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C25/80+D25/20+E25/50+F25/50+G25/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>241</v>
@@ -2367,17 +2289,17 @@
         <v>0</v>
       </c>
       <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G26">
         <v>0</v>
       </c>
@@ -2391,16 +2313,13 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C26/80+D26/20+E26/50+F26/50+G26/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>241</v>
@@ -2409,17 +2328,17 @@
         <v>0</v>
       </c>
       <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G27">
         <v>0</v>
       </c>
@@ -2433,16 +2352,13 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C27/80+D27/20+E27/50+F27/50+G27/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>241</v>
@@ -2451,17 +2367,17 @@
         <v>0</v>
       </c>
       <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G28">
         <v>0</v>
       </c>
@@ -2475,16 +2391,13 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C28/80+D28/20+E28/50+F28/50+G28/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>241</v>
@@ -2517,16 +2430,13 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C29/80+D29/20+E29/50+F29/50+G29/1)/5*2.5,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>241</v>
@@ -2559,16 +2469,13 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C30/80+D30/20+E30/50+F30/50+G30/1)/5*2.5,1)</f>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>241</v>
@@ -2577,17 +2484,17 @@
         <v>0</v>
       </c>
       <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G31">
         <v>0</v>
       </c>
@@ -2601,16 +2508,13 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C31/80+D31/20+E31/50+F31/50+G31/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>241</v>
@@ -2623,7 +2527,7 @@
         <v>17</v>
       </c>
       <c r="E32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F32">
@@ -2643,16 +2547,13 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C32/80+D32/20+E32/50+F32/50+G32/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>241</v>
@@ -2661,11 +2562,11 @@
         <v>64</v>
       </c>
       <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F33">
@@ -2685,16 +2586,13 @@
         <v>0</v>
       </c>
       <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C33/80+D33/20+E33/50+F33/50+G33/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34">
         <v>241</v>
@@ -2727,16 +2625,13 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C34/80+D34/20+E34/50+F34/50+G34/1)/5*2.5,1)</f>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35">
         <v>241</v>
@@ -2769,16 +2664,13 @@
         <v>0</v>
       </c>
       <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C35/80+D35/20+E35/50+F35/50+G35/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36">
         <v>242</v>
@@ -2811,16 +2703,13 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C36/80+D36/20+E36/50+F36/50+G36/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37">
         <v>242</v>
@@ -2853,16 +2742,13 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C37/80+D37/20+E37/50+F37/50+G37/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38">
         <v>242</v>
@@ -2871,17 +2757,17 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:D66" si="4">MIN(ROUNDUP(0*1.1,0),20)</f>
+        <f t="shared" ref="D38:D66" si="3">MIN(ROUNDUP(0*1.1,0),20)</f>
         <v>0</v>
       </c>
       <c r="E38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F38">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G38">
         <v>0</v>
       </c>
@@ -2895,16 +2781,13 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C38/80+D38/20+E38/50+F38/50+G38/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39">
         <v>242</v>
@@ -2913,17 +2796,17 @@
         <v>36</v>
       </c>
       <c r="D39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G39">
         <v>0</v>
       </c>
@@ -2937,16 +2820,13 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C39/80+D39/20+E39/50+F39/50+G39/1)/5*2.5,1)</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40">
         <v>242</v>
@@ -2963,7 +2843,7 @@
         <v>30</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G40">
@@ -2979,16 +2859,13 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C40/80+D40/20+E40/50+F40/50+G40/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41">
         <v>242</v>
@@ -2997,17 +2874,17 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G41">
         <v>0</v>
       </c>
@@ -3021,16 +2898,13 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C41/80+D41/20+E41/50+F41/50+G41/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B42">
         <v>242</v>
@@ -3043,7 +2917,7 @@
         <v>20</v>
       </c>
       <c r="E42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F42">
@@ -3063,16 +2937,13 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C42/80+D42/20+E42/50+F42/50+G42/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B43">
         <v>242</v>
@@ -3085,13 +2956,13 @@
         <v>18</v>
       </c>
       <c r="E43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G43">
         <v>0</v>
       </c>
@@ -3105,16 +2976,13 @@
         <v>0</v>
       </c>
       <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <f t="shared" si="0"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C43/80+D43/20+E43/50+F43/50+G43/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44">
         <v>242</v>
@@ -3123,17 +2991,17 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F44">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G44">
         <v>0</v>
       </c>
@@ -3147,16 +3015,13 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C44/80+D44/20+E44/50+F44/50+G44/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B45">
         <v>242</v>
@@ -3173,7 +3038,7 @@
         <v>28</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G45">
@@ -3189,16 +3054,13 @@
         <v>0</v>
       </c>
       <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C45/80+D45/20+E45/50+F45/50+G45/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B46">
         <v>242</v>
@@ -3207,17 +3069,17 @@
         <v>66</v>
       </c>
       <c r="D46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G46">
         <v>0</v>
       </c>
@@ -3231,16 +3093,13 @@
         <v>0</v>
       </c>
       <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C46/80+D46/20+E46/50+F46/50+G46/1)/5*2.5,1)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B47">
         <v>242</v>
@@ -3273,16 +3132,13 @@
         <v>0</v>
       </c>
       <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="0"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C47/80+D47/20+E47/50+F47/50+G47/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B48">
         <v>242</v>
@@ -3291,17 +3147,17 @@
         <v>70</v>
       </c>
       <c r="D48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G48">
         <v>0</v>
       </c>
@@ -3315,16 +3171,13 @@
         <v>0</v>
       </c>
       <c r="K48">
-        <v>0</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C48/80+D48/20+E48/50+F48/50+G48/1)/5*2.5,1)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B49">
         <v>242</v>
@@ -3333,17 +3186,17 @@
         <v>48</v>
       </c>
       <c r="D49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F49">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G49">
         <v>0</v>
       </c>
@@ -3357,16 +3210,13 @@
         <v>0</v>
       </c>
       <c r="K49">
-        <v>0</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C49/80+D49/20+E49/50+F49/50+G49/1)/5*2.5,1)</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B50">
         <v>242</v>
@@ -3383,7 +3233,7 @@
         <v>28</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G50">
@@ -3399,22 +3249,20 @@
         <v>0</v>
       </c>
       <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C50/80+D50/20+E50/50+F50/50+G50/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B51">
         <v>242</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <f>MIN(ROUNDUP(71*1.1,0),75)</f>
+        <v>75</v>
       </c>
       <c r="D51">
         <f>MIN(ROUNDUP(17*1.1,0),20)</f>
@@ -3441,16 +3289,13 @@
         <v>0</v>
       </c>
       <c r="K51">
-        <v>0</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="0"/>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C51/80+D51/20+E51/50+F51/50+G51/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B52">
         <v>242</v>
@@ -3459,17 +3304,17 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G52">
         <v>0</v>
       </c>
@@ -3483,16 +3328,13 @@
         <v>0</v>
       </c>
       <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C52/80+D52/20+E52/50+F52/50+G52/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53">
         <v>242</v>
@@ -3505,7 +3347,7 @@
         <v>20</v>
       </c>
       <c r="E53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F53">
@@ -3525,16 +3367,13 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <v>0</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C53/80+D53/20+E53/50+F53/50+G53/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B54">
         <v>242</v>
@@ -3547,13 +3386,13 @@
         <v>19</v>
       </c>
       <c r="E54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F54">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F54">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G54">
         <v>0</v>
       </c>
@@ -3567,16 +3406,13 @@
         <v>0</v>
       </c>
       <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C54/80+D54/20+E54/50+F54/50+G54/1)/5*2.5,1)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B55">
         <v>242</v>
@@ -3609,16 +3445,13 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C55/80+D55/20+E55/50+F55/50+G55/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B56">
         <v>242</v>
@@ -3651,16 +3484,13 @@
         <v>0</v>
       </c>
       <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C56/80+D56/20+E56/50+F56/50+G56/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B57">
         <v>242</v>
@@ -3669,17 +3499,17 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F57">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F57">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G57">
         <v>0</v>
       </c>
@@ -3693,16 +3523,13 @@
         <v>0</v>
       </c>
       <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C57/80+D57/20+E57/50+F57/50+G57/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B58">
         <v>242</v>
@@ -3715,13 +3542,13 @@
         <v>20</v>
       </c>
       <c r="E58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F58">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F58">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G58">
         <v>0</v>
       </c>
@@ -3735,16 +3562,13 @@
         <v>0</v>
       </c>
       <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
-        <v>1.9000000000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C58/80+D58/20+E58/50+F58/50+G58/1)/5*2.5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B59">
         <v>242</v>
@@ -3753,17 +3577,17 @@
         <v>0</v>
       </c>
       <c r="D59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F59">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F59">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G59">
         <v>0</v>
       </c>
@@ -3777,16 +3601,13 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C59/80+D59/20+E59/50+F59/50+G59/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B60">
         <v>242</v>
@@ -3795,17 +3616,17 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F60">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F60">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G60">
         <v>0</v>
       </c>
@@ -3819,16 +3640,13 @@
         <v>0</v>
       </c>
       <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C60/80+D60/20+E60/50+F60/50+G60/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B61">
         <v>242</v>
@@ -3861,16 +3679,13 @@
         <v>0</v>
       </c>
       <c r="K61">
-        <v>0</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C61/80+D61/20+E61/50+F61/50+G61/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B62">
         <v>242</v>
@@ -3903,16 +3718,13 @@
         <v>0</v>
       </c>
       <c r="K62">
-        <v>0</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="0"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C62/80+D62/20+E62/50+F62/50+G62/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B63">
         <v>242</v>
@@ -3921,7 +3733,7 @@
         <v>54</v>
       </c>
       <c r="D63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E63">
@@ -3929,7 +3741,7 @@
         <v>26</v>
       </c>
       <c r="F63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G63">
@@ -3945,16 +3757,13 @@
         <v>0</v>
       </c>
       <c r="K63">
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C63/80+D63/20+E63/50+F63/50+G63/1)/5*2.5,1)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B64">
         <v>242</v>
@@ -3987,22 +3796,20 @@
         <v>0</v>
       </c>
       <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C64/80+D64/20+E64/50+F64/50+G64/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B65">
         <v>242</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <f>MIN(ROUNDUP(61*1.1,0),75)</f>
+        <v>68</v>
       </c>
       <c r="D65">
         <f>MIN(ROUNDUP(16*1.1,0),20)</f>
@@ -4029,16 +3836,13 @@
         <v>0</v>
       </c>
       <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="0"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C65/80+D65/20+E65/50+F65/50+G65/1)/5*2.5,1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B66">
         <v>242</v>
@@ -4047,17 +3851,17 @@
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F66">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F66">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="G66">
         <v>0</v>
       </c>
@@ -4071,16 +3875,13 @@
         <v>0</v>
       </c>
       <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="0"/>
+        <f>ROUNDUP(1+(C66/80+D66/20+E66/50+F66/50+G66/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B67">
         <v>242</v>
@@ -4113,22 +3914,20 @@
         <v>0</v>
       </c>
       <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="L67">
-        <f t="shared" ref="L67:L130" si="5">ROUNDUP(1+(C67/80+D67/20+E67/50+F67/50+G67/1+H67/1)/6*2.5,1)</f>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C67/80+D67/20+E67/50+F67/50+G67/1)/5*2.5,1)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B68">
         <v>242</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <f>MIN(ROUNDUP(63*1.1,0),75)</f>
+        <v>70</v>
       </c>
       <c r="D68">
         <f>MIN(ROUNDUP(15*1.1,0),20)</f>
@@ -4139,7 +3938,7 @@
         <v>15</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F130" si="6">MIN(ROUNDUP(0*1.15,0),48)</f>
+        <f t="shared" ref="F68:F130" si="4">MIN(ROUNDUP(0*1.15,0),48)</f>
         <v>0</v>
       </c>
       <c r="G68">
@@ -4155,29 +3954,27 @@
         <v>0</v>
       </c>
       <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="L68">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C68/80+D68/20+E68/50+F68/50+G68/1)/5*2.5,1)</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B69">
         <v>242</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <f>MIN(ROUNDUP(46*1.1,0),75)</f>
+        <v>51</v>
       </c>
       <c r="D69">
         <f>MIN(ROUNDUP(16*1.1,0),20)</f>
         <v>18</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69:E130" si="7">MIN(ROUNDUP(0*1.15,0),48)</f>
+        <f t="shared" ref="E69:E130" si="5">MIN(ROUNDUP(0*1.15,0),48)</f>
         <v>0</v>
       </c>
       <c r="F69">
@@ -4197,16 +3994,13 @@
         <v>0</v>
       </c>
       <c r="K69">
-        <v>0</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C69/80+D69/20+E69/50+F69/50+G69/1)/5*2.5,1)</f>
+        <v>1.9000000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>243</v>
@@ -4239,16 +4033,13 @@
         <v>0</v>
       </c>
       <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C70/80+D70/20+E70/50+F70/50+G70/1)/5*2.5,1)</f>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B71">
         <v>243</v>
@@ -4261,11 +4052,11 @@
         <v>17</v>
       </c>
       <c r="E71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G71">
@@ -4281,16 +4072,13 @@
         <v>0</v>
       </c>
       <c r="K71">
-        <v>0</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="5"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C71/80+D71/20+E71/50+F71/50+G71/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B72">
         <v>243</v>
@@ -4299,15 +4087,15 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <f t="shared" ref="D72:D102" si="8">MIN(ROUNDUP(0*1.1,0),20)</f>
+        <f t="shared" ref="D72:D102" si="6">MIN(ROUNDUP(0*1.1,0),20)</f>
         <v>0</v>
       </c>
       <c r="E72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G72">
@@ -4323,16 +4111,13 @@
         <v>0</v>
       </c>
       <c r="K72">
-        <v>0</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C72/80+D72/20+E72/50+F72/50+G72/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B73">
         <v>243</v>
@@ -4341,15 +4126,15 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G73">
@@ -4365,16 +4150,13 @@
         <v>0</v>
       </c>
       <c r="K73">
-        <v>0</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C73/80+D73/20+E73/50+F73/50+G73/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B74">
         <v>243</v>
@@ -4387,11 +4169,11 @@
         <v>18</v>
       </c>
       <c r="E74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G74">
@@ -4407,16 +4189,13 @@
         <v>0</v>
       </c>
       <c r="K74">
-        <v>0</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="5"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C74/80+D74/20+E74/50+F74/50+G74/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B75">
         <v>243</v>
@@ -4449,16 +4228,13 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>0</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="5"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C75/80+D75/20+E75/50+F75/50+G75/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B76">
         <v>243</v>
@@ -4467,15 +4243,15 @@
         <v>0</v>
       </c>
       <c r="D76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G76">
@@ -4491,16 +4267,13 @@
         <v>0</v>
       </c>
       <c r="K76">
-        <v>0</v>
-      </c>
-      <c r="L76">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C76/80+D76/20+E76/50+F76/50+G76/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B77">
         <v>243</v>
@@ -4533,16 +4306,13 @@
         <v>0</v>
       </c>
       <c r="K77">
-        <v>0</v>
-      </c>
-      <c r="L77">
-        <f t="shared" si="5"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C77/80+D77/20+E77/50+F77/50+G77/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B78">
         <v>243</v>
@@ -4575,16 +4345,13 @@
         <v>0</v>
       </c>
       <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
-        <f t="shared" si="5"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C78/80+D78/20+E78/50+F78/50+G78/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B79">
         <v>243</v>
@@ -4617,16 +4384,13 @@
         <v>0</v>
       </c>
       <c r="K79">
-        <v>0</v>
-      </c>
-      <c r="L79">
-        <f t="shared" si="5"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C79/80+D79/20+E79/50+F79/50+G79/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B80">
         <v>243</v>
@@ -4643,7 +4407,7 @@
         <v>25</v>
       </c>
       <c r="F80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G80">
@@ -4659,16 +4423,13 @@
         <v>0</v>
       </c>
       <c r="K80">
-        <v>0</v>
-      </c>
-      <c r="L80">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C80/80+D80/20+E80/50+F80/50+G80/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B81">
         <v>243</v>
@@ -4677,15 +4438,15 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G81">
@@ -4701,16 +4462,13 @@
         <v>0</v>
       </c>
       <c r="K81">
-        <v>0</v>
-      </c>
-      <c r="L81">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C81/80+D81/20+E81/50+F81/50+G81/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B82">
         <v>243</v>
@@ -4743,16 +4501,13 @@
         <v>0</v>
       </c>
       <c r="K82">
-        <v>0</v>
-      </c>
-      <c r="L82">
-        <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C82/80+D82/20+E82/50+F82/50+G82/1)/5*2.5,1)</f>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B83">
         <v>243</v>
@@ -4769,7 +4524,7 @@
         <v>23</v>
       </c>
       <c r="F83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G83">
@@ -4785,16 +4540,13 @@
         <v>0</v>
       </c>
       <c r="K83">
-        <v>0</v>
-      </c>
-      <c r="L83">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C83/80+D83/20+E83/50+F83/50+G83/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B84">
         <v>243</v>
@@ -4803,15 +4555,15 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G84">
@@ -4827,16 +4579,13 @@
         <v>0</v>
       </c>
       <c r="K84">
-        <v>0</v>
-      </c>
-      <c r="L84">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C84/80+D84/20+E84/50+F84/50+G84/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B85">
         <v>243</v>
@@ -4845,15 +4594,15 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G85">
@@ -4869,16 +4618,13 @@
         <v>0</v>
       </c>
       <c r="K85">
-        <v>0</v>
-      </c>
-      <c r="L85">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C85/80+D85/20+E85/50+F85/50+G85/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B86">
         <v>243</v>
@@ -4911,16 +4657,13 @@
         <v>0</v>
       </c>
       <c r="K86">
-        <v>0</v>
-      </c>
-      <c r="L86">
-        <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C86/80+D86/20+E86/50+F86/50+G86/1)/5*2.5,1)</f>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B87">
         <v>243</v>
@@ -4953,16 +4696,13 @@
         <v>0</v>
       </c>
       <c r="K87">
-        <v>0</v>
-      </c>
-      <c r="L87">
-        <f t="shared" si="5"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C87/80+D87/20+E87/50+F87/50+G87/1)/5*2.5,1)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B88">
         <v>243</v>
@@ -4975,11 +4715,11 @@
         <v>17</v>
       </c>
       <c r="E88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G88">
@@ -4995,16 +4735,13 @@
         <v>0</v>
       </c>
       <c r="K88">
-        <v>0</v>
-      </c>
-      <c r="L88">
-        <f t="shared" si="5"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C88/80+D88/20+E88/50+F88/50+G88/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B89">
         <v>243</v>
@@ -5017,11 +4754,11 @@
         <v>18</v>
       </c>
       <c r="E89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G89">
@@ -5037,16 +4774,13 @@
         <v>0</v>
       </c>
       <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="L89">
-        <f t="shared" si="5"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C89/80+D89/20+E89/50+F89/50+G89/1)/5*2.5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B90">
         <v>243</v>
@@ -5079,16 +4813,13 @@
         <v>0</v>
       </c>
       <c r="K90">
-        <v>0</v>
-      </c>
-      <c r="L90">
-        <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C90/80+D90/20+E90/50+F90/50+G90/1)/5*2.5,1)</f>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B91">
         <v>243</v>
@@ -5097,15 +4828,15 @@
         <v>57</v>
       </c>
       <c r="D91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G91">
@@ -5121,16 +4852,13 @@
         <v>0</v>
       </c>
       <c r="K91">
-        <v>0</v>
-      </c>
-      <c r="L91">
-        <f t="shared" si="5"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C91/80+D91/20+E91/50+F91/50+G91/1)/5*2.5,1)</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B92">
         <v>243</v>
@@ -5163,16 +4891,13 @@
         <v>0</v>
       </c>
       <c r="K92">
-        <v>0</v>
-      </c>
-      <c r="L92">
-        <f t="shared" si="5"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C92/80+D92/20+E92/50+F92/50+G92/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B93">
         <v>243</v>
@@ -5185,11 +4910,11 @@
         <v>18</v>
       </c>
       <c r="E93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G93">
@@ -5205,16 +4930,13 @@
         <v>0</v>
       </c>
       <c r="K93">
-        <v>0</v>
-      </c>
-      <c r="L93">
-        <f t="shared" si="5"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C93/80+D93/20+E93/50+F93/50+G93/1)/5*2.5,1)</f>
+        <v>1.9000000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B94">
         <v>243</v>
@@ -5247,16 +4969,13 @@
         <v>0</v>
       </c>
       <c r="K94">
-        <v>0</v>
-      </c>
-      <c r="L94">
-        <f t="shared" si="5"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C94/80+D94/20+E94/50+F94/50+G94/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B95">
         <v>243</v>
@@ -5289,16 +5008,13 @@
         <v>0</v>
       </c>
       <c r="K95">
-        <v>0</v>
-      </c>
-      <c r="L95">
-        <f t="shared" si="5"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C95/80+D95/20+E95/50+F95/50+G95/1)/5*2.5,1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B96">
         <v>243</v>
@@ -5307,15 +5023,15 @@
         <v>0</v>
       </c>
       <c r="D96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G96">
@@ -5331,16 +5047,13 @@
         <v>0</v>
       </c>
       <c r="K96">
-        <v>0</v>
-      </c>
-      <c r="L96">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C96/80+D96/20+E96/50+F96/50+G96/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B97">
         <v>243</v>
@@ -5349,15 +5062,15 @@
         <v>0</v>
       </c>
       <c r="D97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G97">
@@ -5373,16 +5086,13 @@
         <v>0</v>
       </c>
       <c r="K97">
-        <v>0</v>
-      </c>
-      <c r="L97">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C97/80+D97/20+E97/50+F97/50+G97/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B98">
         <v>243</v>
@@ -5395,7 +5105,7 @@
         <v>18</v>
       </c>
       <c r="E98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F98">
@@ -5415,16 +5125,13 @@
         <v>0</v>
       </c>
       <c r="K98">
-        <v>0</v>
-      </c>
-      <c r="L98">
-        <f t="shared" si="5"/>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C98/80+D98/20+E98/50+F98/50+G98/1)/5*2.5,1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B99">
         <v>243</v>
@@ -5433,15 +5140,15 @@
         <v>0</v>
       </c>
       <c r="D99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G99">
@@ -5457,16 +5164,13 @@
         <v>0</v>
       </c>
       <c r="K99">
-        <v>0</v>
-      </c>
-      <c r="L99">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C99/80+D99/20+E99/50+F99/50+G99/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B100">
         <v>243</v>
@@ -5475,15 +5179,15 @@
         <v>0</v>
       </c>
       <c r="D100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G100">
@@ -5499,16 +5203,13 @@
         <v>0</v>
       </c>
       <c r="K100">
-        <v>0</v>
-      </c>
-      <c r="L100">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C100/80+D100/20+E100/50+F100/50+G100/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B101">
         <v>243</v>
@@ -5541,16 +5242,13 @@
         <v>0</v>
       </c>
       <c r="K101">
-        <v>0</v>
-      </c>
-      <c r="L101">
-        <f t="shared" si="5"/>
-        <v>2.3000000000000003</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C101/80+D101/20+E101/50+F101/50+G101/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B102">
         <v>243</v>
@@ -5559,15 +5257,15 @@
         <v>0</v>
       </c>
       <c r="D102">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G102">
@@ -5583,16 +5281,13 @@
         <v>0</v>
       </c>
       <c r="K102">
-        <v>0</v>
-      </c>
-      <c r="L102">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C102/80+D102/20+E102/50+F102/50+G102/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B103">
         <v>244</v>
@@ -5625,16 +5320,13 @@
         <v>0</v>
       </c>
       <c r="K103">
-        <v>0</v>
-      </c>
-      <c r="L103">
-        <f t="shared" si="5"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C103/80+D103/20+E103/50+F103/50+G103/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B104">
         <v>244</v>
@@ -5643,15 +5335,15 @@
         <v>0</v>
       </c>
       <c r="D104">
-        <f t="shared" ref="D104:D133" si="9">MIN(ROUNDUP(0*1.1,0),20)</f>
+        <f t="shared" ref="D104:D133" si="7">MIN(ROUNDUP(0*1.1,0),20)</f>
         <v>0</v>
       </c>
       <c r="E104">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F104">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G104">
@@ -5667,16 +5359,13 @@
         <v>0</v>
       </c>
       <c r="K104">
-        <v>0</v>
-      </c>
-      <c r="L104">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C104/80+D104/20+E104/50+F104/50+G104/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B105">
         <v>244</v>
@@ -5693,7 +5382,7 @@
         <v>33</v>
       </c>
       <c r="F105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G105">
@@ -5709,16 +5398,13 @@
         <v>0</v>
       </c>
       <c r="K105">
-        <v>0</v>
-      </c>
-      <c r="L105">
-        <f t="shared" si="5"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C105/80+D105/20+E105/50+F105/50+G105/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B106">
         <v>244</v>
@@ -5727,7 +5413,7 @@
         <v>54</v>
       </c>
       <c r="D106">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E106">
@@ -5735,7 +5421,7 @@
         <v>29</v>
       </c>
       <c r="F106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G106">
@@ -5751,16 +5437,13 @@
         <v>0</v>
       </c>
       <c r="K106">
-        <v>0</v>
-      </c>
-      <c r="L106">
-        <f t="shared" si="5"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C106/80+D106/20+E106/50+F106/50+G106/1)/5*2.5,1)</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B107">
         <v>244</v>
@@ -5769,15 +5452,15 @@
         <v>0</v>
       </c>
       <c r="D107">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G107">
@@ -5793,22 +5476,20 @@
         <v>0</v>
       </c>
       <c r="K107">
-        <v>0</v>
-      </c>
-      <c r="L107">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C107/80+D107/20+E107/50+F107/50+G107/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B108">
         <v>244</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <f>MIN(ROUNDUP(72*1.1,0),75)</f>
+        <v>75</v>
       </c>
       <c r="D108">
         <f>MIN(ROUNDUP(19*1.1,0),20)</f>
@@ -5835,16 +5516,13 @@
         <v>0</v>
       </c>
       <c r="K108">
-        <v>0</v>
-      </c>
-      <c r="L108">
-        <f t="shared" si="5"/>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C108/80+D108/20+E108/50+F108/50+G108/1)/5*2.5,1)</f>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B109">
         <v>244</v>
@@ -5877,16 +5555,13 @@
         <v>0</v>
       </c>
       <c r="K109">
-        <v>0</v>
-      </c>
-      <c r="L109">
-        <f t="shared" si="5"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C109/80+D109/20+E109/50+F109/50+G109/1)/5*2.5,1)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B110">
         <v>244</v>
@@ -5903,7 +5578,7 @@
         <v>17</v>
       </c>
       <c r="F110">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G110">
@@ -5919,16 +5594,13 @@
         <v>0</v>
       </c>
       <c r="K110">
-        <v>0</v>
-      </c>
-      <c r="L110">
-        <f t="shared" si="5"/>
-        <v>1.9000000000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C110/80+D110/20+E110/50+F110/50+G110/1)/5*2.5,1)</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B111">
         <v>244</v>
@@ -5961,16 +5633,13 @@
         <v>0</v>
       </c>
       <c r="K111">
-        <v>0</v>
-      </c>
-      <c r="L111">
-        <f t="shared" si="5"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C111/80+D111/20+E111/50+F111/50+G111/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B112">
         <v>244</v>
@@ -6003,22 +5672,20 @@
         <v>0</v>
       </c>
       <c r="K112">
-        <v>0</v>
-      </c>
-      <c r="L112">
-        <f t="shared" si="5"/>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C112/80+D112/20+E112/50+F112/50+G112/1)/5*2.5,1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B113">
         <v>244</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <f>MIN(ROUNDUP(57*1.1,0),75)</f>
+        <v>63</v>
       </c>
       <c r="D113">
         <f>MIN(ROUNDUP(16*1.1,0),20)</f>
@@ -6045,16 +5712,13 @@
         <v>0</v>
       </c>
       <c r="K113">
-        <v>0</v>
-      </c>
-      <c r="L113">
-        <f t="shared" si="5"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C113/80+D113/20+E113/50+F113/50+G113/1)/5*2.5,1)</f>
+        <v>2.3000000000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B114">
         <v>244</v>
@@ -6063,7 +5727,7 @@
         <v>71</v>
       </c>
       <c r="D114">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E114">
@@ -6071,7 +5735,7 @@
         <v>32</v>
       </c>
       <c r="F114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G114">
@@ -6087,16 +5751,13 @@
         <v>0</v>
       </c>
       <c r="K114">
-        <v>0</v>
-      </c>
-      <c r="L114">
-        <f t="shared" si="5"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C114/80+D114/20+E114/50+F114/50+G114/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B115">
         <v>244</v>
@@ -6105,7 +5766,7 @@
         <v>66</v>
       </c>
       <c r="D115">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E115">
@@ -6113,7 +5774,7 @@
         <v>43</v>
       </c>
       <c r="F115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G115">
@@ -6129,16 +5790,13 @@
         <v>0</v>
       </c>
       <c r="K115">
-        <v>0</v>
-      </c>
-      <c r="L115">
-        <f t="shared" si="5"/>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C115/80+D115/20+E115/50+F115/50+G115/1)/5*2.5,1)</f>
+        <v>1.9000000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B116">
         <v>244</v>
@@ -6147,15 +5805,15 @@
         <v>61</v>
       </c>
       <c r="D116">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E116">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G116">
@@ -6171,22 +5829,20 @@
         <v>0</v>
       </c>
       <c r="K116">
-        <v>0</v>
-      </c>
-      <c r="L116">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C116/80+D116/20+E116/50+F116/50+G116/1)/5*2.5,1)</f>
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B117">
         <v>244</v>
       </c>
       <c r="C117">
-        <v>49</v>
+        <f>MIN(ROUNDUP(60*1.1,0),75)</f>
+        <v>66</v>
       </c>
       <c r="D117">
         <f>MIN(ROUNDUP(16*1.1,0),20)</f>
@@ -6213,16 +5869,13 @@
         <v>0</v>
       </c>
       <c r="K117">
-        <v>0</v>
-      </c>
-      <c r="L117">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C117/80+D117/20+E117/50+F117/50+G117/1)/5*2.5,1)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B118">
         <v>244</v>
@@ -6232,7 +5885,7 @@
         <v>49</v>
       </c>
       <c r="D118">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E118">
@@ -6240,7 +5893,7 @@
         <v>33</v>
       </c>
       <c r="F118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G118">
@@ -6256,16 +5909,13 @@
         <v>0</v>
       </c>
       <c r="K118">
-        <v>0</v>
-      </c>
-      <c r="L118">
-        <f t="shared" si="5"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C118/80+D118/20+E118/50+F118/50+G118/1)/5*2.5,1)</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B119">
         <v>244</v>
@@ -6274,15 +5924,15 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E119">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G119">
@@ -6298,16 +5948,13 @@
         <v>0</v>
       </c>
       <c r="K119">
-        <v>0</v>
-      </c>
-      <c r="L119">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C119/80+D119/20+E119/50+F119/50+G119/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B120">
         <v>244</v>
@@ -6340,16 +5987,13 @@
         <v>0</v>
       </c>
       <c r="K120">
-        <v>0</v>
-      </c>
-      <c r="L120">
-        <f t="shared" si="5"/>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C120/80+D120/20+E120/50+F120/50+G120/1)/5*2.5,1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B121">
         <v>244</v>
@@ -6358,15 +6002,15 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E121">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G121">
@@ -6382,16 +6026,13 @@
         <v>0</v>
       </c>
       <c r="K121">
-        <v>0</v>
-      </c>
-      <c r="L121">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C121/80+D121/20+E121/50+F121/50+G121/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B122">
         <v>244</v>
@@ -6409,7 +6050,7 @@
         <v>32</v>
       </c>
       <c r="F122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G122">
@@ -6425,16 +6066,13 @@
         <v>0</v>
       </c>
       <c r="K122">
-        <v>0</v>
-      </c>
-      <c r="L122">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C122/80+D122/20+E122/50+F122/50+G122/1)/5*2.5,1)</f>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B123">
         <v>244</v>
@@ -6444,15 +6082,15 @@
         <v>24</v>
       </c>
       <c r="D123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G123">
@@ -6468,22 +6106,19 @@
         <v>0</v>
       </c>
       <c r="K123">
-        <v>0</v>
-      </c>
-      <c r="L123">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C123/80+D123/20+E123/50+F123/50+G123/1)/5*2.5,1)</f>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B124">
         <v>244</v>
       </c>
       <c r="C124">
-        <f t="shared" ref="C124:C132" si="10">MIN(ROUNDUP(0*1.1,0),78)</f>
+        <f t="shared" ref="C124:C132" si="8">MIN(ROUNDUP(0*1.1,0),78)</f>
         <v>0</v>
       </c>
       <c r="D124">
@@ -6495,7 +6130,7 @@
         <v>15</v>
       </c>
       <c r="F124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G124">
@@ -6511,16 +6146,13 @@
         <v>0</v>
       </c>
       <c r="K124">
-        <v>0</v>
-      </c>
-      <c r="L124">
-        <f t="shared" si="5"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C124/80+D124/20+E124/50+F124/50+G124/1)/5*2.5,1)</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B125">
         <v>244</v>
@@ -6530,15 +6162,15 @@
         <v>71</v>
       </c>
       <c r="D125">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G125">
@@ -6554,34 +6186,31 @@
         <v>0</v>
       </c>
       <c r="K125">
-        <v>0</v>
-      </c>
-      <c r="L125">
-        <f t="shared" si="5"/>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C125/80+D125/20+E125/50+F125/50+G125/1)/5*2.5,1)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B126">
         <v>244</v>
       </c>
       <c r="C126">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D126">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E126">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G126">
@@ -6597,16 +6226,13 @@
         <v>0</v>
       </c>
       <c r="K126">
-        <v>0</v>
-      </c>
-      <c r="L126">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C126/80+D126/20+E126/50+F126/50+G126/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B127">
         <v>244</v>
@@ -6616,7 +6242,7 @@
         <v>49</v>
       </c>
       <c r="D127">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E127">
@@ -6624,7 +6250,7 @@
         <v>32</v>
       </c>
       <c r="F127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G127">
@@ -6640,22 +6266,19 @@
         <v>0</v>
       </c>
       <c r="K127">
-        <v>0</v>
-      </c>
-      <c r="L127">
-        <f t="shared" si="5"/>
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C127/80+D127/20+E127/50+F127/50+G127/1)/5*2.5,1)</f>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B128">
         <v>244</v>
       </c>
       <c r="C128">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D128">
@@ -6663,11 +6286,11 @@
         <v>7</v>
       </c>
       <c r="E128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G128">
@@ -6683,16 +6306,13 @@
         <v>0</v>
       </c>
       <c r="K128">
-        <v>0</v>
-      </c>
-      <c r="L128">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C128/80+D128/20+E128/50+F128/50+G128/1)/5*2.5,1)</f>
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B129">
         <v>244</v>
@@ -6702,15 +6322,15 @@
         <v>57</v>
       </c>
       <c r="D129">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E129">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G129">
@@ -6726,34 +6346,31 @@
         <v>0</v>
       </c>
       <c r="K129">
-        <v>0</v>
-      </c>
-      <c r="L129">
-        <f t="shared" si="5"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C129/80+D129/20+E129/50+F129/50+G129/1)/5*2.5,1)</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B130">
         <v>244</v>
       </c>
       <c r="C130">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D130">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E130">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F130">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G130">
@@ -6769,16 +6386,13 @@
         <v>0</v>
       </c>
       <c r="K130">
-        <v>0</v>
-      </c>
-      <c r="L130">
-        <f t="shared" si="5"/>
+        <f>ROUNDUP(1+(C130/80+D130/20+E130/50+F130/50+G130/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B131">
         <v>244</v>
@@ -6788,7 +6402,7 @@
         <v>46</v>
       </c>
       <c r="D131">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E131">
@@ -6796,7 +6410,7 @@
         <v>44</v>
       </c>
       <c r="F131">
-        <f t="shared" ref="F131:F134" si="11">MIN(ROUNDUP(0*1.15,0),48)</f>
+        <f t="shared" ref="F131:F134" si="9">MIN(ROUNDUP(0*1.15,0),48)</f>
         <v>0</v>
       </c>
       <c r="G131">
@@ -6812,36 +6426,33 @@
         <v>0</v>
       </c>
       <c r="K131">
-        <v>0</v>
-      </c>
-      <c r="L131">
-        <f t="shared" ref="L131:L134" si="12">ROUNDUP(1+(C131/80+D131/20+E131/50+F131/50+G131/1+H131/1)/6*2.5,1)</f>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.45">
+        <f>ROUNDUP(1+(C131/80+D131/20+E131/50+F131/50+G131/1)/5*2.5,1)</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B132">
         <v>244</v>
       </c>
       <c r="C132">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D132">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <f t="shared" ref="E132:E134" si="10">MIN(ROUNDUP(0*1.15,0),48)</f>
+        <v>0</v>
+      </c>
+      <c r="F132">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E132">
-        <f t="shared" ref="E132:E134" si="13">MIN(ROUNDUP(0*1.15,0),48)</f>
-        <v>0</v>
-      </c>
-      <c r="F132">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
       <c r="G132">
         <v>0</v>
       </c>
@@ -6855,16 +6466,13 @@
         <v>0</v>
       </c>
       <c r="K132">
-        <v>0</v>
-      </c>
-      <c r="L132">
-        <f t="shared" si="12"/>
+        <f>ROUNDUP(1+(C132/80+D132/20+E132/50+F132/50+G132/1)/5*2.5,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B133">
         <v>244</v>
@@ -6874,17 +6482,17 @@
         <v>46</v>
       </c>
       <c r="D133">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F133">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E133">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="F133">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
       <c r="G133">
         <v>0</v>
       </c>
@@ -6898,16 +6506,13 @@
         <v>0</v>
       </c>
       <c r="K133">
-        <v>0</v>
-      </c>
-      <c r="L133">
-        <f t="shared" si="12"/>
+        <f>ROUNDUP(1+(C133/80+D133/20+E133/50+F133/50+G133/1)/5*2.5,1)</f>
         <v>1.3</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B134">
         <v>244</v>
@@ -6921,11 +6526,11 @@
         <v>20</v>
       </c>
       <c r="E134">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F134">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G134">
@@ -6941,21 +6546,12 @@
         <v>0</v>
       </c>
       <c r="K134">
-        <v>0</v>
-      </c>
-      <c r="L134">
-        <f t="shared" si="12"/>
-        <v>1.7000000000000002</v>
+        <f>ROUNDUP(1+(C134/80+D134/20+E134/50+F134/50+G134/1)/5*2.5,1)</f>
+        <v>1.9000000000000001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L134">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="244"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K134"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Restanta 1 Prob & Stat
</commit_message>
<xml_diff>
--- a/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/ProbabilityStatistics/results/Tabel_Prob_Stat.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1311,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="G94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6346,7 +6346,7 @@
         <v>243</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D103">
         <f t="shared" si="13"/>
@@ -6378,11 +6378,11 @@
       </c>
       <c r="M103">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.3125</v>
       </c>
       <c r="N103">
         <f t="shared" si="9"/>
-        <v>1.8</v>
+        <v>2.1124999999999998</v>
       </c>
       <c r="P103">
         <v>7</v>

</xml_diff>